<commit_message>
data added to worksheet
</commit_message>
<xml_diff>
--- a/NCU-PAYS-COR-JUNE 19 2024 (003).xlsx
+++ b/NCU-PAYS-COR-JUNE 19 2024 (003).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011" filterPrivacy="true"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="PAYS MAY 30 2024 (2)" sheetId="1" r:id="rId1"/>
   </sheets>
@@ -35,10 +35,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="3">
+  <numFmts count="1">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;J$&quot;* #,##0.00_-;-&quot;J$&quot;* #,##0.00_-;_-&quot;J$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -402,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -418,7 +416,7 @@
         <v>Registered</v>
       </c>
       <c r="D1" t="str">
-        <v xml:space="preserve">Semester Cost </v>
+        <v>SemesterCost</v>
       </c>
       <c r="E1" t="str">
         <v>Semester</v>
@@ -464,7 +462,7 @@
         <v>117324779</v>
       </c>
       <c r="B3" t="str">
-        <v>SLB-RLOS-131580</v>
+        <v>SLB-RLOS-123385</v>
       </c>
       <c r="C3" t="str">
         <v>YES</v>
@@ -603,10 +601,62 @@
         <v>2023</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>100291708</v>
+      </c>
+      <c r="B9" t="str">
+        <v>SLB-RLOS-123385</v>
+      </c>
+      <c r="C9" t="str">
+        <v>YES</v>
+      </c>
+      <c r="D9">
+        <v>181946.18</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>3.79</v>
+      </c>
+      <c r="G9" t="str">
+        <v/>
+      </c>
+      <c r="H9">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>117324779</v>
+      </c>
+      <c r="B10" t="str">
+        <v>SLB-RLOS-131580</v>
+      </c>
+      <c r="C10" t="str">
+        <v>YES</v>
+      </c>
+      <c r="D10">
+        <v>105062.45</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="str">
+        <v/>
+      </c>
+      <c r="H10">
+        <v>2023</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
installed mysql, modified payscoreexcel, added sql file
</commit_message>
<xml_diff>
--- a/NCU-PAYS-COR-JUNE 19 2024 (003).xlsx
+++ b/NCU-PAYS-COR-JUNE 19 2024 (003).xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -462,7 +462,7 @@
         <v>117324779</v>
       </c>
       <c r="B3" t="str">
-        <v>SLB-RLOS-123385</v>
+        <v>SLB-RLOS-131580</v>
       </c>
       <c r="C3" t="str">
         <v>YES</v>
@@ -534,16 +534,16 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>101053070</v>
+        <v>110732120</v>
       </c>
       <c r="B6" t="str">
-        <v>SLB-RLOS-131776</v>
+        <v>SLB-RLOS-129449</v>
       </c>
       <c r="C6" t="str">
         <v>YES</v>
       </c>
       <c r="D6">
-        <v>30918.62</v>
+        <v>516608.67999999993</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -578,85 +578,36 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8">
-        <v>110732120</v>
-      </c>
-      <c r="B8" t="str">
-        <v>SLB-RLOS-129449</v>
-      </c>
-      <c r="C8" t="str">
-        <v>YES</v>
-      </c>
-      <c r="D8">
-        <v>516608.67999999993</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>2023</v>
-      </c>
-    </row>
     <row r="9">
-      <c r="A9" t="str">
-        <v>100291708</v>
+      <c r="A9">
+        <v>127645999</v>
       </c>
       <c r="B9" t="str">
-        <v>SLB-RLOS-123385</v>
+        <v>SLB-RLOS-141000</v>
       </c>
       <c r="C9" t="str">
         <v>YES</v>
       </c>
       <c r="D9">
-        <v>181946.18</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>3.79</v>
+        <v>0</v>
       </c>
       <c r="G9" t="str">
         <v/>
       </c>
       <c r="H9">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>117324779</v>
-      </c>
-      <c r="B10" t="str">
-        <v>SLB-RLOS-131580</v>
-      </c>
-      <c r="C10" t="str">
-        <v>YES</v>
-      </c>
-      <c r="D10">
-        <v>105062.45</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" t="str">
-        <v/>
-      </c>
-      <c r="H10">
         <v>2023</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>